<commit_message>
Todas las interfaces hechas.
</commit_message>
<xml_diff>
--- a/Carpeta de Proyecto/Actores.xlsx
+++ b/Carpeta de Proyecto/Actores.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programacion\GitHub\Gym\Carpeta de Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BC0A5EE6-56D8-4C25-8D39-B497A00EFBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A6A353-0B12-42B8-B000-2F83591A8A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="0" yWindow="1716" windowWidth="9096" windowHeight="10644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Actores</t>
   </si>
@@ -72,11 +73,81 @@
     <t>Notificación de cuotas a vencer y/o vencidas.
 Modificación de alumnos.</t>
   </si>
+  <si>
+    <t>Casos de uso</t>
+  </si>
+  <si>
+    <t>Caso</t>
+  </si>
+  <si>
+    <t>Descripción</t>
+  </si>
+  <si>
+    <t>Caso de uso</t>
+  </si>
+  <si>
+    <t>Actor principal</t>
+  </si>
+  <si>
+    <t>Personal involucrado e intereses</t>
+  </si>
+  <si>
+    <t>Precondiciones</t>
+  </si>
+  <si>
+    <t>Garantías de éxito</t>
+  </si>
+  <si>
+    <t>Frecuencia</t>
+  </si>
+  <si>
+    <t>El estado del empleado cambiará de Activo a Inactivo, no aparecerá más en ningún plan como profesor, y si tenía acceso al programa, se bloqueará usuario y clave.</t>
+  </si>
+  <si>
+    <t>Módulos</t>
+  </si>
+  <si>
+    <t>Asistencia</t>
+  </si>
+  <si>
+    <t>Registro</t>
+  </si>
+  <si>
+    <t>Pagos</t>
+  </si>
+  <si>
+    <t>Caja</t>
+  </si>
+  <si>
+    <t>Planes</t>
+  </si>
+  <si>
+    <t>Empleados</t>
+  </si>
+  <si>
+    <t>Cerrar Sesión</t>
+  </si>
+  <si>
+    <t>Dueño, Encargados, Sistema de caja</t>
+  </si>
+  <si>
+    <t>Total de dinero en caja
+Total de dinero en el sistema 
+Fecha
+Estado
+Empleado/dueño (quien abrió la caja)</t>
+  </si>
+  <si>
+    <t>Sesión del actor iniciada Ok. Caja Abierta.</t>
+  </si>
+  <si>
+    <t>Siempre que la caja esté abierta y el usuario intente cerrar sesión sin cerrar la caja antes.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -107,7 +178,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,20 +186,55 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -443,184 +549,205 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F22"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H7" sqref="H1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B1" s="3" t="s">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-    </row>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B2" s="1" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="H1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2" t="s">
+      <c r="C2" s="4"/>
+      <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="1" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="H3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="H4" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="H5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="H6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="H7" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="2" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B12" s="4"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B14" s="4"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2" t="s">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="2"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -635,4 +762,215 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F95A70-BF0F-4AD7-BEF2-FE9069C147F4}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C8" sqref="A2:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+    </row>
+    <row r="8" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="6"/>
+      <c r="C8" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="11"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="7"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="11"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="30">
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="A10:E10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C5:E5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Se modifica la base de datos, y por ende las historias de usuario, ya que hay campos que no estaban contemplados, necesarios para las conexiones, o el desarollo de la bdd.
</commit_message>
<xml_diff>
--- a/Carpeta de Proyecto/Actores.xlsx
+++ b/Carpeta de Proyecto/Actores.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programacion\GitHub\Gym\Carpeta de Proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59A6A353-0B12-42B8-B000-2F83591A8A14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B449E156-3F5A-4776-8A8F-FF1891920A42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1716" windowWidth="9096" windowHeight="10644" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="117">
   <si>
     <t>Actores</t>
   </si>
@@ -143,12 +144,273 @@
   <si>
     <t>Siempre que la caja esté abierta y el usuario intente cerrar sesión sin cerrar la caja antes.</t>
   </si>
+  <si>
+    <t>Base de datos por módulo</t>
+  </si>
+  <si>
+    <t>alumnos</t>
+  </si>
+  <si>
+    <t>alternativo</t>
+  </si>
+  <si>
+    <t>mail</t>
+  </si>
+  <si>
+    <t>plan</t>
+  </si>
+  <si>
+    <t>observaciones</t>
+  </si>
+  <si>
+    <t>id_empleado</t>
+  </si>
+  <si>
+    <t>telefono</t>
+  </si>
+  <si>
+    <t>nombre_apellido</t>
+  </si>
+  <si>
+    <t>tipo_documento</t>
+  </si>
+  <si>
+    <t>tipo_documento_id</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>estado</t>
+  </si>
+  <si>
+    <t>clase</t>
+  </si>
+  <si>
+    <t>empleados</t>
+  </si>
+  <si>
+    <t>num_dni</t>
+  </si>
+  <si>
+    <t>tipo_empleado</t>
+  </si>
+  <si>
+    <t>empleado_id</t>
+  </si>
+  <si>
+    <t>tipo_empleado_id</t>
+  </si>
+  <si>
+    <t>jornadas</t>
+  </si>
+  <si>
+    <t>lunes</t>
+  </si>
+  <si>
+    <t>martes</t>
+  </si>
+  <si>
+    <t>miercoles</t>
+  </si>
+  <si>
+    <t>jueves</t>
+  </si>
+  <si>
+    <t>viernes</t>
+  </si>
+  <si>
+    <t>sabados</t>
+  </si>
+  <si>
+    <t>todos</t>
+  </si>
+  <si>
+    <t>jornada</t>
+  </si>
+  <si>
+    <t>costos</t>
+  </si>
+  <si>
+    <t>cuotas</t>
+  </si>
+  <si>
+    <t>alumno_id</t>
+  </si>
+  <si>
+    <t>estado_plan_id</t>
+  </si>
+  <si>
+    <t>activo</t>
+  </si>
+  <si>
+    <t>inactivo</t>
+  </si>
+  <si>
+    <t>baja</t>
+  </si>
+  <si>
+    <t>al dia</t>
+  </si>
+  <si>
+    <t>deudor</t>
+  </si>
+  <si>
+    <t>actual</t>
+  </si>
+  <si>
+    <t>modificado</t>
+  </si>
+  <si>
+    <t>fecha_inscripcion</t>
+  </si>
+  <si>
+    <t>fecha_pago</t>
+  </si>
+  <si>
+    <t>recursividad</t>
+  </si>
+  <si>
+    <t>caja_abierta</t>
+  </si>
+  <si>
+    <t>caja_cerrada</t>
+  </si>
+  <si>
+    <t>fecha_apertura</t>
+  </si>
+  <si>
+    <t>apertura_caja</t>
+  </si>
+  <si>
+    <t>cierre_caja</t>
+  </si>
+  <si>
+    <t>apertura_caja_id</t>
+  </si>
+  <si>
+    <t>monto_apertura_cash</t>
+  </si>
+  <si>
+    <t>fecha_cierre</t>
+  </si>
+  <si>
+    <t>monto_cierre_caja</t>
+  </si>
+  <si>
+    <t>monto_cierre_efectivo</t>
+  </si>
+  <si>
+    <t>dueño</t>
+  </si>
+  <si>
+    <t>estados_cuotas</t>
+  </si>
+  <si>
+    <t>estados_plan</t>
+  </si>
+  <si>
+    <t>Tipos_empleado</t>
+  </si>
+  <si>
+    <t>estados_empleado</t>
+  </si>
+  <si>
+    <t>estados_alumno</t>
+  </si>
+  <si>
+    <t>tipos_documento</t>
+  </si>
+  <si>
+    <t>cierre_Caja</t>
+  </si>
+  <si>
+    <t>sistema encendido</t>
+  </si>
+  <si>
+    <t>tipo_doc</t>
+  </si>
+  <si>
+    <t>empleado</t>
+  </si>
+  <si>
+    <t>alumno</t>
+  </si>
+  <si>
+    <t>apertura</t>
+  </si>
+  <si>
+    <t>asignacion_id</t>
+  </si>
+  <si>
+    <t>programador</t>
+  </si>
+  <si>
+    <t>Requerimientos previos a crear cada registro</t>
+  </si>
+  <si>
+    <t>plan_id</t>
+  </si>
+  <si>
+    <t>pagos</t>
+  </si>
+  <si>
+    <t>importe</t>
+  </si>
+  <si>
+    <t>vigente</t>
+  </si>
+  <si>
+    <t>paga</t>
+  </si>
+  <si>
+    <t>adeudada</t>
+  </si>
+  <si>
+    <t>estados_facturacion</t>
+  </si>
+  <si>
+    <t>estado_facturacion</t>
+  </si>
+  <si>
+    <t>Activo</t>
+  </si>
+  <si>
+    <t>Inactivo</t>
+  </si>
+  <si>
+    <t>Carpeta Médica</t>
+  </si>
+  <si>
+    <t>Vacaciones</t>
+  </si>
+  <si>
+    <t>Baja</t>
+  </si>
+  <si>
+    <t>Otros</t>
+  </si>
+  <si>
+    <t>estado_alumno_id</t>
+  </si>
+  <si>
+    <t>estado_empleado_id</t>
+  </si>
+  <si>
+    <t>estado_cuota_id</t>
+  </si>
+  <si>
+    <t>concepto_id</t>
+  </si>
+  <si>
+    <t>usuario_id</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,8 +425,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,8 +447,80 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -201,14 +543,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -236,6 +661,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,202 +981,202 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:H22"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H7" sqref="H1:H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5" t="s">
+      <c r="C1" s="31"/>
+      <c r="D1" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
       <c r="H1" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="3" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
       <c r="H2" s="2" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
       <c r="H3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="29"/>
+      <c r="F4" s="29"/>
       <c r="H4" s="2" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
       <c r="H5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
       <c r="H6" s="2" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
       <c r="H7" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="29"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" spans="2:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="3" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="29"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="29"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="29"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="29"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="29"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="29"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="29"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="4"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
     </row>
     <row r="18" spans="2:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3" t="s">
+      <c r="C18" s="29"/>
+      <c r="D18" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
+      <c r="B19" s="29"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -768,8 +1197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57F95A70-BF0F-4AD7-BEF2-FE9069C147F4}">
   <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="A2:E8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -778,164 +1207,164 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="8"/>
-      <c r="C2" s="8" t="s">
+      <c r="B2" s="34"/>
+      <c r="C2" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="32"/>
+      <c r="C3" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="9" t="s">
+      <c r="B4" s="32"/>
+      <c r="C4" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="10" t="s">
+      <c r="B5" s="32"/>
+      <c r="C5" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="32"/>
+      <c r="C6" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
     </row>
     <row r="7" spans="1:5" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="10" t="s">
+      <c r="B7" s="32"/>
+      <c r="C7" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
     </row>
     <row r="8" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="10" t="s">
+      <c r="B8" s="32"/>
+      <c r="C8" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="7"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="33"/>
+      <c r="C11" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="7"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="A12" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="7"/>
-      <c r="E12" s="7"/>
+      <c r="B12" s="37"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="A13" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
-      <c r="E13" s="7"/>
+      <c r="B13" s="37"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
+      <c r="B14" s="37"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
+      <c r="B15" s="37"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="11" t="s">
+      <c r="A16" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
+      <c r="A17" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="7"/>
+      <c r="B17" s="37"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -973,4 +1402,459 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{350D31F0-8C7C-4337-9F92-0AF531B55F42}">
+  <dimension ref="A1:N24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="15.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.44140625" style="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.77734375" style="11" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.21875" style="11" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.88671875" style="11" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="15.44140625" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H2" s="11" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="M3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="L4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E6" s="22"/>
+      <c r="G6" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="J8" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="L9" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="N9" s="39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="N10" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="K12" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="10" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" s="38" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="38"/>
+      <c r="C19" s="38"/>
+      <c r="D19" s="38"/>
+      <c r="E19" s="38"/>
+      <c r="F19" s="38"/>
+      <c r="G19" s="38"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C22" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="E22" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B23" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E24" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A19:G19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>